<commit_message>
creando modal para registrar clientes
</commit_message>
<xml_diff>
--- a/PERMISOS.xlsx
+++ b/PERMISOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ProyectoCredipyme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B734CC-1FA2-4254-A283-0E1460D9D456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3357E4-9D54-4C51-A3DE-8EBFE7C847C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="2415" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PERMISOS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>ÁREA</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>CREDITOS_ESTADOS</t>
+  </si>
+  <si>
+    <t>CLIENTES</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,8 +436,8 @@
         <v>4</v>
       </c>
       <c r="E3" t="str">
-        <f>CONCATENATE("insert into permisos (modulo,submodulo) values (","'",B3,"'",",","'",C3,"'",")",";")</f>
-        <v>insert into permisos (modulo,submodulo) values ('SISTEMA','HOME');</v>
+        <f>CONCATENATE("insert into permiso(modulo,submodulo) values (","'",B3,"'",",","'",C3,"'",")",";")</f>
+        <v>insert into permiso(modulo,submodulo) values ('SISTEMA','HOME');</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -445,8 +448,8 @@
         <v>2</v>
       </c>
       <c r="E5" t="str">
-        <f>CONCATENATE("insert into permisos (modulo,submodulo) values (","'",B5,"'",",","'",C5,"'",")",";")</f>
-        <v>insert into permisos (modulo,submodulo) values ('USUARIOS','GESTION');</v>
+        <f t="shared" ref="E5:E6" si="0">CONCATENATE("insert into permiso(modulo,submodulo) values (","'",B5,"'",",","'",C5,"'",")",";")</f>
+        <v>insert into permiso(modulo,submodulo) values ('USUARIOS','GESTION');</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -457,35 +460,20 @@
         <v>7</v>
       </c>
       <c r="E6" t="str">
-        <f>CONCATENATE("insert into permisos (modulo,submodulo) values (","'",B6,"'",",","'",C6,"'",")",";")</f>
-        <v>insert into permisos (modulo,submodulo) values ('USUARIOS','PERMISOS');</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
+        <f t="shared" si="0"/>
+        <v>insert into permiso(modulo,submodulo) values ('USUARIOS','PERMISOS');</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" ref="E8:E14" si="0">CONCATENATE("insert into permisos (modulo,submodulo) values (","'",B8,"'",",","'",C8,"'",")",";")</f>
-        <v>insert into permisos (modulo,submodulo) values ('MANTENIMIENTO','USUARIOS_CARGOS');</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into permisos (modulo,submodulo) values ('MANTENIMIENTO','USUARIOS_AGENCIAS');</v>
+        <f>CONCATENATE("insert into permiso(modulo,submodulo) values (","'",B8,"'",",","'",C8,"'",")",";")</f>
+        <v>insert into permiso(modulo,submodulo) values ('CLIENTES','GESTION');</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -493,11 +481,11 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into permisos (modulo,submodulo) values ('MANTENIMIENTO','USUARIOS_PERMISOS');</v>
+        <f t="shared" ref="E10:E16" si="1">CONCATENATE("insert into permiso(modulo,submodulo) values (","'",B10,"'",",","'",C10,"'",")",";")</f>
+        <v>insert into permiso(modulo,submodulo) values ('MANTENIMIENTO','USUARIOS_CARGOS');</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -505,11 +493,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into permisos (modulo,submodulo) values ('MANTENIMIENTO','CREDITOS_SECTORES');</v>
+        <f t="shared" si="1"/>
+        <v>insert into permiso(modulo,submodulo) values ('MANTENIMIENTO','USUARIOS_AGENCIAS');</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -517,11 +505,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into permisos (modulo,submodulo) values ('MANTENIMIENTO','CREDITOS_PRODUCTOS');</v>
+        <f t="shared" si="1"/>
+        <v>insert into permiso(modulo,submodulo) values ('MANTENIMIENTO','USUARIOS_PERMISOS');</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -529,11 +517,11 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into permisos (modulo,submodulo) values ('MANTENIMIENTO','CREDITOS_TIPOS');</v>
+        <f t="shared" si="1"/>
+        <v>insert into permiso(modulo,submodulo) values ('MANTENIMIENTO','CREDITOS_SECTORES');</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -541,11 +529,35 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into permiso(modulo,submodulo) values ('MANTENIMIENTO','CREDITOS_PRODUCTOS');</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into permiso(modulo,submodulo) values ('MANTENIMIENTO','CREDITOS_TIPOS');</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into permisos (modulo,submodulo) values ('MANTENIMIENTO','CREDITOS_ESTADOS');</v>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into permiso(modulo,submodulo) values ('MANTENIMIENTO','CREDITOS_ESTADOS');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>